<commit_message>
bind all plankton data after cleaning up spreadsheets
</commit_message>
<xml_diff>
--- a/data/biology/counts/09202019.xlsx
+++ b/data/biology/counts/09202019.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="26122"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19420" windowHeight="11020" activeTab="5"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19420" windowHeight="11020" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="411" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1024" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1018" uniqueCount="104">
   <si>
     <t>date</t>
   </si>
@@ -325,21 +325,6 @@
     <t>zoea1.3</t>
   </si>
   <si>
-    <t>n = 39</t>
-  </si>
-  <si>
-    <t>n = 44</t>
-  </si>
-  <si>
-    <t>chth?</t>
-  </si>
-  <si>
-    <t>n = 23</t>
-  </si>
-  <si>
-    <t>n = 29</t>
-  </si>
-  <si>
     <t>marine mite</t>
   </si>
   <si>
@@ -353,9 +338,6 @@
   </si>
   <si>
     <t>polychaete.nonspionid</t>
-  </si>
-  <si>
-    <t>n = 31</t>
   </si>
   <si>
     <t>pandalus.spp</t>
@@ -475,8 +457,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -499,9 +483,11 @@
     <xf numFmtId="14" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -816,8 +802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1258,7 +1244,7 @@
         <v>128</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>31</v>
@@ -1461,7 +1447,7 @@
         <v>16</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="H22" s="5" t="s">
         <v>18</v>
@@ -1522,7 +1508,7 @@
         <v>83</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="I24" s="5">
         <v>2</v>
@@ -1606,7 +1592,7 @@
         <v>16</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="H27" s="5" t="s">
         <v>31</v>
@@ -1664,7 +1650,7 @@
         <v>16</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="H29" s="5" t="s">
         <v>95</v>
@@ -1751,7 +1737,7 @@
         <v>16</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="H32" s="5" t="s">
         <v>95</v>
@@ -1761,9 +1747,7 @@
       </c>
     </row>
     <row r="34" spans="1:1">
-      <c r="A34" s="9" t="s">
-        <v>106</v>
-      </c>
+      <c r="A34" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1781,7 +1765,7 @@
   <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2957,9 +2941,7 @@
       </c>
     </row>
     <row r="42" spans="1:9">
-      <c r="A42" s="9" t="s">
-        <v>96</v>
-      </c>
+      <c r="A42" s="9"/>
     </row>
   </sheetData>
   <sortState ref="A2:J27">
@@ -2980,8 +2962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="H47" sqref="H47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3173,9 +3155,7 @@
       <c r="I6" s="7">
         <v>56</v>
       </c>
-      <c r="J6" s="7" t="s">
-        <v>98</v>
-      </c>
+      <c r="J6" s="7"/>
       <c r="K6" s="7"/>
     </row>
     <row r="7" spans="1:11">
@@ -4166,7 +4146,7 @@
         <v>61</v>
       </c>
       <c r="H40" s="7" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="I40" s="5">
         <v>4</v>
@@ -4282,7 +4262,7 @@
         <v>83</v>
       </c>
       <c r="H44" s="7" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="I44" s="5">
         <v>6</v>
@@ -4299,9 +4279,7 @@
       <c r="M45" s="7"/>
     </row>
     <row r="46" spans="1:13">
-      <c r="A46" s="9" t="s">
-        <v>97</v>
-      </c>
+      <c r="A46" s="9"/>
     </row>
   </sheetData>
   <sortState ref="A1:M36">
@@ -4321,8 +4299,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5036,9 +5014,7 @@
       <c r="A25" s="4"/>
     </row>
     <row r="26" spans="1:9">
-      <c r="A26" s="11" t="s">
-        <v>99</v>
-      </c>
+      <c r="A26" s="11"/>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="4"/>
@@ -5061,8 +5037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5948,9 +5924,7 @@
       </c>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="9" t="s">
-        <v>100</v>
-      </c>
+      <c r="A32" s="9"/>
     </row>
   </sheetData>
   <sortState ref="A1:K26">
@@ -5970,7 +5944,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>

</xml_diff>